<commit_message>
Aline corrected sample weight issue
Aline generated w_sampleweight separately and tested using Turkumanistan data, there's no issue on missing sampleweight for indicators anymore.
</commit_message>
<xml_diff>
--- a/Codebook_MICS.xlsx
+++ b/Codebook_MICS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/sneelsen_worldbank_org/Documents/Projects/UHC/04 STC/Haozheyi/World Bank/MEASURE UHC DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/sneelsen_worldbank_org/Documents/Projects/UHC/04 STC/Haozheyi/World Bank/MEASURE UHC DATA/STATA/DO/SC/06_Prepare_MICS6/MICS6_DW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{5DA5234B-8C42-4549-B683-AFC33CB4F9F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5530A5CD-26B6-4669-88F1-5FCCF2E3AC88}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{5DA5234B-8C42-4549-B683-AFC33CB4F9F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{85A62FB2-6CBF-488C-80D6-D9450DC2EF66}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{73496108-0DF4-4D51-854A-96DF35928E2E}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{73496108-0DF4-4D51-854A-96DF35928E2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook_DHS" sheetId="1" state="hidden" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Codebook_DHS!$A$1:$N$132</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Codebook_MICS!$A$1:$N$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Codebook_MICS!$A$1:$N$114</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="730">
   <si>
     <t>DHS Country Code</t>
   </si>
@@ -2666,6 +2666,7 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2720,7 +2721,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2737,10 +2737,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7953,7 +7949,7 @@
         <f>VLOOKUP(B132,MICS_vars!A:A,1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="E132" s="94"/>
+      <c r="E132" s="76"/>
       <c r="G132" s="1" t="s">
         <v>0</v>
       </c>
@@ -9057,15 +9053,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA4135F-04ED-4914-A652-21B0822352F3}">
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="3" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" customWidth="1"/>
+    <col min="2" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" customWidth="1"/>
     <col min="8" max="11" width="10.7109375" customWidth="1"/>
@@ -12172,9 +12167,7 @@
       <c r="B84" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C84" s="16" t="s">
-        <v>693</v>
-      </c>
+      <c r="C84" s="16"/>
       <c r="D84" s="16" t="s">
         <v>693</v>
       </c>
@@ -13267,7 +13260,7 @@
       <c r="N114" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N110" xr:uid="{04A01C68-77EC-4758-BA68-84CC49919051}"/>
+  <autoFilter ref="A1:N114" xr:uid="{04A01C68-77EC-4758-BA68-84CC49919051}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13304,124 +13297,124 @@
         <v>692</v>
       </c>
       <c r="C1" s="75"/>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="83" t="s">
         <v>691</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="85" t="s">
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="86" t="s">
         <v>690</v>
       </c>
-      <c r="R1" s="86"/>
-      <c r="S1" s="87" t="s">
+      <c r="R1" s="87"/>
+      <c r="S1" s="88" t="s">
         <v>689</v>
       </c>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
-      <c r="AG1" s="87"/>
-      <c r="AH1" s="88" t="s">
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
+      <c r="W1" s="88"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="88"/>
+      <c r="AA1" s="88"/>
+      <c r="AB1" s="88"/>
+      <c r="AC1" s="88"/>
+      <c r="AD1" s="88"/>
+      <c r="AE1" s="88"/>
+      <c r="AF1" s="88"/>
+      <c r="AG1" s="88"/>
+      <c r="AH1" s="89" t="s">
         <v>688</v>
       </c>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="88"/>
-      <c r="AK1" s="88"/>
-      <c r="AL1" s="88"/>
-      <c r="AM1" s="88"/>
-      <c r="AN1" s="88"/>
-      <c r="AO1" s="88"/>
-      <c r="AP1" s="88"/>
-      <c r="AQ1" s="88"/>
+      <c r="AI1" s="89"/>
+      <c r="AJ1" s="89"/>
+      <c r="AK1" s="89"/>
+      <c r="AL1" s="89"/>
+      <c r="AM1" s="89"/>
+      <c r="AN1" s="89"/>
+      <c r="AO1" s="89"/>
+      <c r="AP1" s="89"/>
+      <c r="AQ1" s="89"/>
     </row>
     <row r="2" spans="2:43" s="67" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B2" s="65" t="s">
         <v>687</v>
       </c>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="90" t="s">
         <v>686</v>
       </c>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
       <c r="N2" s="73" t="s">
         <v>685</v>
       </c>
-      <c r="O2" s="90" t="s">
+      <c r="O2" s="91" t="s">
         <v>684</v>
       </c>
-      <c r="P2" s="91"/>
+      <c r="P2" s="92"/>
       <c r="Q2" s="72" t="s">
         <v>683</v>
       </c>
       <c r="R2" s="71" t="s">
         <v>682</v>
       </c>
-      <c r="S2" s="92" t="s">
+      <c r="S2" s="93" t="s">
         <v>681</v>
       </c>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
       <c r="V2" s="70" t="s">
         <v>680</v>
       </c>
-      <c r="W2" s="93" t="s">
+      <c r="W2" s="94" t="s">
         <v>679</v>
       </c>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="93"/>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="76" t="s">
+      <c r="X2" s="94"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="94"/>
+      <c r="AA2" s="77" t="s">
         <v>678</v>
       </c>
-      <c r="AB2" s="76"/>
-      <c r="AC2" s="76"/>
-      <c r="AD2" s="76"/>
-      <c r="AE2" s="76"/>
-      <c r="AF2" s="76"/>
+      <c r="AB2" s="77"/>
+      <c r="AC2" s="77"/>
+      <c r="AD2" s="77"/>
+      <c r="AE2" s="77"/>
+      <c r="AF2" s="77"/>
       <c r="AG2" s="69" t="s">
         <v>677</v>
       </c>
-      <c r="AH2" s="77" t="s">
+      <c r="AH2" s="78" t="s">
         <v>676</v>
       </c>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="78"/>
-      <c r="AK2" s="79"/>
-      <c r="AL2" s="80" t="s">
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="80"/>
+      <c r="AL2" s="81" t="s">
         <v>675</v>
       </c>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="81" t="s">
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="82" t="s">
         <v>674</v>
       </c>
-      <c r="AP2" s="81"/>
+      <c r="AP2" s="82"/>
       <c r="AQ2" s="68" t="s">
         <v>673</v>
       </c>

</xml_diff>